<commit_message>
fix(export): purge template images and re-insert logo via ExcelJS for iOS
</commit_message>
<xml_diff>
--- a/public/templates/shaken_template.xlsx
+++ b/public/templates/shaken_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaydo\appdevelope\HayashiDr\moto-invoice\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E896597F-61E8-48BD-BD28-9B1F749A267F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980947DE-6400-4E5D-AAD2-7CDF059B06F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,28 +37,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </valueMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1104,33 +1082,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1191,8 +1142,35 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1276,70 +1254,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1666,13 +1580,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B8A382-8351-4233-ABBC-379BB1C9197E}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
     <col min="2" max="2" width="45.26953125" customWidth="1"/>
     <col min="3" max="3" width="21.1796875" customWidth="1"/>
     <col min="4" max="4" width="10.453125" style="1" customWidth="1"/>
@@ -1682,14 +1596,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
     </row>
     <row r="2" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="62"/>
@@ -1711,9 +1625,9 @@
       <c r="C3" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
@@ -1723,9 +1637,9 @@
       <c r="C4" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
@@ -1737,9 +1651,9 @@
       <c r="C5" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="s">
@@ -1749,9 +1663,9 @@
       <c r="C6" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -1765,10 +1679,10 @@
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="69"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="6" t="s">
         <v>2</v>
       </c>
@@ -1783,10 +1697,10 @@
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="71"/>
+      <c r="C9" s="93"/>
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
       <c r="F9" s="10">
@@ -1796,10 +1710,10 @@
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="73"/>
+      <c r="C10" s="95"/>
       <c r="D10" s="12"/>
       <c r="E10" s="13"/>
       <c r="F10" s="14">
@@ -1809,10 +1723,10 @@
     </row>
     <row r="11" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="73"/>
+      <c r="C11" s="95"/>
       <c r="D11" s="12"/>
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
@@ -2106,11 +2020,11 @@
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="82" t="s">
+      <c r="A37" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="83"/>
-      <c r="C37" s="84"/>
+      <c r="B37" s="74"/>
+      <c r="C37" s="75"/>
       <c r="D37" s="45"/>
       <c r="E37" s="46"/>
       <c r="F37" s="48">
@@ -2119,11 +2033,11 @@
       </c>
     </row>
     <row r="38" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="85" t="s">
+      <c r="A38" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="86"/>
-      <c r="C38" s="87"/>
+      <c r="B38" s="77"/>
+      <c r="C38" s="78"/>
       <c r="D38" s="47"/>
       <c r="E38" s="39"/>
       <c r="F38" s="48">
@@ -2132,11 +2046,11 @@
       </c>
     </row>
     <row r="39" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="88" t="s">
+      <c r="A39" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="89"/>
-      <c r="C39" s="90"/>
+      <c r="B39" s="80"/>
+      <c r="C39" s="81"/>
       <c r="D39" s="49"/>
       <c r="E39" s="50"/>
       <c r="F39" s="51">
@@ -2176,10 +2090,10 @@
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="91" t="s">
+      <c r="D42" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="91"/>
+      <c r="E42" s="82"/>
       <c r="F42" s="55">
         <f>F41*1.1</f>
         <v>0</v>
@@ -2189,73 +2103,80 @@
       <c r="A43" s="56"/>
       <c r="B43" s="56"/>
       <c r="C43" s="67"/>
-      <c r="D43" s="92" t="s">
+      <c r="D43" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="81"/>
+      <c r="E43" s="72"/>
       <c r="F43" s="55">
         <f>SUM(F42+F13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="97" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="B44" s="93"/>
-      <c r="C44" s="94"/>
-      <c r="D44" s="80" t="s">
+      <c r="A44" s="88"/>
+      <c r="B44" s="84"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="E44" s="81"/>
+      <c r="E44" s="72"/>
       <c r="F44" s="55"/>
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="98"/>
-      <c r="B45" s="77" t="s">
+      <c r="A45" s="89"/>
+      <c r="B45" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="78"/>
-      <c r="D45" s="80" t="s">
+      <c r="C45" s="69"/>
+      <c r="D45" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="81"/>
+      <c r="E45" s="72"/>
       <c r="F45" s="55"/>
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="98"/>
-      <c r="B46" s="95" t="s">
+      <c r="A46" s="89"/>
+      <c r="B46" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="96"/>
-      <c r="D46" s="80" t="s">
+      <c r="C46" s="87"/>
+      <c r="D46" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="81"/>
+      <c r="E46" s="72"/>
       <c r="F46" s="57">
         <f>SUM(F43-F45)-F44</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="98"/>
-      <c r="B47" s="79" t="s">
+      <c r="A47" s="89"/>
+      <c r="B47" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="79"/>
+      <c r="C47" s="70"/>
     </row>
     <row r="48" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="98"/>
-      <c r="B48" s="79"/>
-      <c r="C48" s="79"/>
+      <c r="A48" s="89"/>
+      <c r="B48" s="70"/>
+      <c r="C48" s="70"/>
     </row>
     <row r="49" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="98"/>
-      <c r="B49" s="79"/>
-      <c r="C49" s="79"/>
+      <c r="A49" s="89"/>
+      <c r="B49" s="70"/>
+      <c r="C49" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B47:C49"/>
     <mergeCell ref="D45:E45"/>
@@ -2269,15 +2190,6 @@
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.25" right="0.25" top="5.9027777777777776E-3" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>